<commit_message>
cambios al archivo de casos de prueba
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoFinal-MariaCelesteParedes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8166D3-5A77-4D16-A7B0-DBE601C79D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A02E120-0C75-4063-A6D8-009E151FD425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="143">
   <si>
     <t>ID</t>
   </si>
@@ -33,9 +33,6 @@
     <t>TC-001</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>TC-002</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>TC-015</t>
   </si>
   <si>
-    <t>TC-016</t>
-  </si>
-  <si>
     <t>Nombre del Proyecto:</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
     <t>Alta</t>
   </si>
   <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
     <t>Registro</t>
   </si>
   <si>
@@ -166,6 +166,294 @@
   </si>
   <si>
     <t>Mostrar la pantalla principal confirmando el acceso exitoso.</t>
+  </si>
+  <si>
+    <t>Registro con Contraseña Débil (Negativo)</t>
+  </si>
+  <si>
+    <t>Verificar el mensaje de error al usar una contraseña que NO cumple con los requisitos mínimos de seguridad.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Email: prueba@invalida.com, Contraseña: 123</t>
+  </si>
+  <si>
+    <t>Validación de contraseña mínima.</t>
+  </si>
+  <si>
+    <t>1. Abrir la app. 2. Seleccionar "Registrarse". 3. Ingresar Email y Contraseña débil. 4. Presionar "Iniciar sesión".</t>
+  </si>
+  <si>
+    <t>Mostrar un mensaje de error claro indicando que la contraseña no cumple con las condiciones de seguridad mínimas.</t>
+  </si>
+  <si>
+    <t>Inicio de Sesión con Credenciales Inválidas (Negativo)</t>
+  </si>
+  <si>
+    <t>Verificar que se muestre un mensaje de error al intentar iniciar sesión con credenciales no válidas.</t>
+  </si>
+  <si>
+    <t>Email: incorrecto@test.com, Contraseña: mala_pass</t>
+  </si>
+  <si>
+    <t>Acceso denegado con error.</t>
+  </si>
+  <si>
+    <t>1. Abrir la app. 2. Seleccionar "Iniciar sesión". 3. Ingresar credenciales no válidas. 4. Presionar "Iniciar sesión".</t>
+  </si>
+  <si>
+    <t>Mostrar el mensaje de error: "Usuario o contraseña incorrectos".</t>
+  </si>
+  <si>
+    <t>Acceder a Galería para Publicación</t>
+  </si>
+  <si>
+    <t>Publicación</t>
+  </si>
+  <si>
+    <t>Verificar el acceso directo a la galería del dispositivo al tocar el botón de publicación.</t>
+  </si>
+  <si>
+    <t>El usuario debe estar logueado y tener permisos de acceso a la galería.</t>
+  </si>
+  <si>
+    <t>Acceso directo a galería.</t>
+  </si>
+  <si>
+    <t>1. Iniciar sesión. 2. Tocar el botón de publicación (el botón '+').</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar la galería del dispositivo para la selección de contenido.</t>
+  </si>
+  <si>
+    <t>Publicar una Única Foto con Descripción</t>
+  </si>
+  <si>
+    <t>Verificar la publicación de una foto seleccionada desde la galería, incluyendo un texto descriptivo.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, con una foto en la galería lista para publicar.</t>
+  </si>
+  <si>
+    <t>Foto: img_vacaciones.jpg, Descripción: "Gran día en la playa!"</t>
+  </si>
+  <si>
+    <t>Publicación de foto simple con texto.</t>
+  </si>
+  <si>
+    <t>1. Tocar '+', seleccionar una única foto. 2. Tocar "Siguiente". 3. Ingresar el texto descriptivo. 4. Presionar "Compartir" (o Publicar).</t>
+  </si>
+  <si>
+    <t>La foto debe aparecer en el feed del usuario con el texto descriptivo añadido.</t>
+  </si>
+  <si>
+    <t>Publicar un Único Video Corto</t>
+  </si>
+  <si>
+    <t>Verificar la publicación de un único video corto seleccionado de la galería.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, con un video corto disponible.</t>
+  </si>
+  <si>
+    <t>Video: vid_corto_10s.mp4, Descripción: (Opcional)</t>
+  </si>
+  <si>
+    <t>Publicación de video corto simple.</t>
+  </si>
+  <si>
+    <t>1. Tocar '+', seleccionar un único video corto. 2. Seguir los pasos de publicación. 3. Presionar "Compartir".</t>
+  </si>
+  <si>
+    <t>El video corto debe aparecer en el feed del usuario y reproducirse correctamente.</t>
+  </si>
+  <si>
+    <t>Intento de Selección Múltiple (Negativo)</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema NO permite la selección de más de un elemento (foto o video) para la publicación simultánea.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, con al menos dos elementos en la galería.</t>
+  </si>
+  <si>
+    <t>Seleccionar foto_1.jpg y foto_2.jpg.</t>
+  </si>
+  <si>
+    <t>Restricción de selección única.</t>
+  </si>
+  <si>
+    <t>1. Tocar '+', intentar seleccionar dos o más elementos.</t>
+  </si>
+  <si>
+    <t>El sistema solo debe permitir la selección de un único elemento (foto o video) a la vez para continuar con la publicación.</t>
+  </si>
+  <si>
+    <t>Dar 'Me Gusta' por Primera Vez</t>
+  </si>
+  <si>
+    <t>Interacción (Like)</t>
+  </si>
+  <si>
+    <t>Verificar que al tocar el icono de corazón, el contador aumente y el icono cambie de color.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, publicación visible en el feed, la publicación NO debe tener un 'Me Gusta' previo del usuario.</t>
+  </si>
+  <si>
+    <t>Publicación ID: P-001</t>
+  </si>
+  <si>
+    <t>Acción de "Me Gusta" inicial.</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación P-001. 2. Tocar el icono de corazón (vacío).</t>
+  </si>
+  <si>
+    <t>El contador de "Me Gusta" debe aumentar en una unidad, y el icono debe cambiar de vacío (blanco) a lleno (rojo).</t>
+  </si>
+  <si>
+    <t>Eliminar 'Me Gusta' (Dislike)</t>
+  </si>
+  <si>
+    <t>Verificar que al volver a tocar el icono, se elimine el 'Me Gusta' y el contador disminuya.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, publicación visible en el feed, la publicación debe tener un 'Me Gusta' previo del usuario (icono rojo/lleno).</t>
+  </si>
+  <si>
+    <t>Eliminación de "Me Gusta".</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación P-001. 2. Tocar el icono de corazón (rojo/lleno).</t>
+  </si>
+  <si>
+    <t>El contador de "Me Gusta" debe disminuir en una unidad, y el icono debe volver a su estado vacío (blanco).</t>
+  </si>
+  <si>
+    <t>Doble 'Me Gusta' (Validación de Estado)</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema mantenga un solo 'Me Gusta' aunque se toque el icono repetidamente.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, publicación sin 'Me Gusta' previo del usuario.</t>
+  </si>
+  <si>
+    <t>Publicación ID: P-002</t>
+  </si>
+  <si>
+    <t>Estado estable del contador.</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación P-002. 2. Tocar el icono de corazón (vacío). 3. Tocar el icono de corazón (rojo/lleno) inmediatamente de nuevo.</t>
+  </si>
+  <si>
+    <t>El contador de "Me Gusta" debe aumentar en 1 en el primer toque y luego volver al conteo original en el segundo toque (neto: 0 cambios).</t>
+  </si>
+  <si>
+    <t>Guardar Publicación por Primera Vez</t>
+  </si>
+  <si>
+    <t>Interacción (Guardar)</t>
+  </si>
+  <si>
+    <t>Verificar que al tocar el icono de 'Guardar', el icono cambie de estado y la publicación se guarde.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, publicación visible en el feed, la publicación NO debe estar guardada previamente.</t>
+  </si>
+  <si>
+    <t>Publicación ID: P-003</t>
+  </si>
+  <si>
+    <t>Acción de "Guardar" inicial.</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación P-003. 2. Tocar el icono de 'Guardar' (vacío).</t>
+  </si>
+  <si>
+    <t>El icono de 'Guardar' debe cambiar de vacío a lleno (rojo), indicando que la publicación ha sido guardada.</t>
+  </si>
+  <si>
+    <t>Acceder a Publicación Guardada</t>
+  </si>
+  <si>
+    <t>Verificar que una publicación guardada sea accesible en la sección de Publicaciones Guardadas del perfil.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, Publicación ID: P-003 previamente guardada (CP11).</t>
+  </si>
+  <si>
+    <t>Verificación de acceso a lista.</t>
+  </si>
+  <si>
+    <t>1. Ir al perfil del usuario. 2. Acceder a la sección de "Publicaciones Guardadas". 3. Buscar la publicación P-003.</t>
+  </si>
+  <si>
+    <t>La publicación P-003 debe aparecer y ser visible dentro de la sección de Publicaciones Guardadas.</t>
+  </si>
+  <si>
+    <t>Eliminar Publicación Guardada</t>
+  </si>
+  <si>
+    <t>Verificar que al volver a tocar el icono de 'Guardar' se elimine el guardado y el icono cambie de estado.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, Publicación ID: P-003 previamente guardada (icono rojo/lleno).</t>
+  </si>
+  <si>
+    <t>Eliminación de "Guardar".</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación P-003 (guardada). 2. Tocar el icono de 'Guardar' (rojo/lleno) nuevamente. 3. (Opcional) Verificar la sección de Guardadas.</t>
+  </si>
+  <si>
+    <t>El icono de 'Guardar' debe volver a su estado vacío, y la publicación P-003 debe desaparecer de la sección de Publicaciones Guardadas.</t>
+  </si>
+  <si>
+    <t>Velocidad de Guardado de Publicación (Performance)</t>
+  </si>
+  <si>
+    <t>Rendimiento (Guardar)</t>
+  </si>
+  <si>
+    <t>Verificar que la acción de guardar una publicación se realice de forma ágil.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, publicación visible.</t>
+  </si>
+  <si>
+    <t>Publicación ID: P-004</t>
+  </si>
+  <si>
+    <t>Tiempo de respuesta de la acción.</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación P-004. 2. Tocar el icono de 'Guardar'. 3. Medir el tiempo hasta el cambio de estado del icono.</t>
+  </si>
+  <si>
+    <t>El cambio de estado del icono de 'Guardar' (vacío a lleno) debe ser inmediato (perceptualmente ágil, ej. menos de 1 segundo).</t>
+  </si>
+  <si>
+    <t>Velocidad de Recuperación de Lista Guardada (Performance)</t>
+  </si>
+  <si>
+    <t>Verificar que la lista de publicaciones guardadas se recupere de forma ágil.</t>
+  </si>
+  <si>
+    <t>Usuario logueado, con al menos 10 publicaciones guardadas previamente.</t>
+  </si>
+  <si>
+    <t>Tiempo de carga de la lista.</t>
+  </si>
+  <si>
+    <t>1. Ir al perfil del usuario. 2. Acceder a la sección de "Publicaciones Guardadas". 3. Medir el tiempo de carga de la lista.</t>
+  </si>
+  <si>
+    <t>La lista de publicaciones guardadas debe mostrarse de forma águil y rápida (perceptualmente instantánea o muy corta, ej. menos de 2 segundos).</t>
   </si>
 </sst>
 </file>
@@ -661,7 +949,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,8 +963,8 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
     <col min="13" max="13" width="27.28515625" customWidth="1"/>
   </cols>
@@ -684,44 +972,44 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
@@ -732,40 +1020,40 @@
         <v>0</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="M8" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="105" x14ac:dyDescent="0.25">
@@ -788,10 +1076,10 @@
         <v>43</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>44</v>
@@ -802,248 +1090,524 @@
       <c r="K9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+        <v>7</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
@@ -1188,9 +1752,7 @@
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>

</xml_diff>

<commit_message>
agrege caso 2 y 3 con su respectiva evidencia
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoFinal-MariaCelesteParedes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A02E120-0C75-4063-A6D8-009E151FD425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFE7C96-7F85-45A2-A17F-7092D92DDFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -147,18 +147,12 @@
     <t>Registro</t>
   </si>
   <si>
-    <t>Registro Exitoso</t>
-  </si>
-  <si>
     <t>Verificar el registro exitoso de una nueva cuenta con email y contraseña válidos.</t>
   </si>
   <si>
     <t>1. No debe existir una cuenta previamente registrada con el email de prueba.</t>
   </si>
   <si>
-    <t>1.Email:                                             2. Contraseña:</t>
-  </si>
-  <si>
     <t>Registro con credenciales válidas.</t>
   </si>
   <si>
@@ -168,42 +162,15 @@
     <t>Mostrar la pantalla principal confirmando el acceso exitoso.</t>
   </si>
   <si>
-    <t>Registro con Contraseña Débil (Negativo)</t>
-  </si>
-  <si>
     <t>Verificar el mensaje de error al usar una contraseña que NO cumple con los requisitos mínimos de seguridad.</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Email: prueba@invalida.com, Contraseña: 123</t>
-  </si>
-  <si>
     <t>Validación de contraseña mínima.</t>
   </si>
   <si>
-    <t>1. Abrir la app. 2. Seleccionar "Registrarse". 3. Ingresar Email y Contraseña débil. 4. Presionar "Iniciar sesión".</t>
-  </si>
-  <si>
-    <t>Mostrar un mensaje de error claro indicando que la contraseña no cumple con las condiciones de seguridad mínimas.</t>
-  </si>
-  <si>
-    <t>Inicio de Sesión con Credenciales Inválidas (Negativo)</t>
-  </si>
-  <si>
-    <t>Verificar que se muestre un mensaje de error al intentar iniciar sesión con credenciales no válidas.</t>
-  </si>
-  <si>
-    <t>Email: incorrecto@test.com, Contraseña: mala_pass</t>
-  </si>
-  <si>
-    <t>Acceso denegado con error.</t>
-  </si>
-  <si>
-    <t>1. Abrir la app. 2. Seleccionar "Iniciar sesión". 3. Ingresar credenciales no válidas. 4. Presionar "Iniciar sesión".</t>
-  </si>
-  <si>
     <t>Mostrar el mensaje de error: "Usuario o contraseña incorrectos".</t>
   </si>
   <si>
@@ -454,13 +421,73 @@
   </si>
   <si>
     <t>La lista de publicaciones guardadas debe mostrarse de forma águil y rápida (perceptualmente instantánea o muy corta, ej. menos de 2 segundos).</t>
+  </si>
+  <si>
+    <t>1.Email:         tarjeteriafinaperu@gmail.com                                    2. Contraseña: 1234maria</t>
+  </si>
+  <si>
+    <t>NO PASO</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-001</t>
+  </si>
+  <si>
+    <t>Registro con contraseña Exitoso con correo electronico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro con Contraseña Exitoso con numero de celular </t>
+  </si>
+  <si>
+    <t>Verificar el registro exitoso de un numero de celular y contraseña válidos.</t>
+  </si>
+  <si>
+    <t>1. No debe existir una cuenta previamente registrada con el numero de prueba.</t>
+  </si>
+  <si>
+    <t>Numero de celular: 51+921297961  Contraseña: 324667</t>
+  </si>
+  <si>
+    <t>1. Abrir la app. 2. Seleccionar "Registrarse". 3. Ingresar numero y Contraseña débil. 4. Presionar "Iniciar sesión".</t>
+  </si>
+  <si>
+    <t>1. Abrir la app.                 2. Seleccionar "Registrarse".                    3. Ingresar numero y Contraseña                      4. Presionar "Iniciar sesión".</t>
+  </si>
+  <si>
+    <t>PASO</t>
+  </si>
+  <si>
+    <t>Mostrar la pantalla inmediatamente añade una foto en el perfil.</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro con Contraseña Débil con numero de celular </t>
+  </si>
+  <si>
+    <t>Numero de celular: 51+921297961  Contraseña: 32466</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-003</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+  <si>
+    <t>No permite continuar la prueba por boton de siguiente.</t>
+  </si>
+  <si>
+    <t>Muestra aviso de informacion.</t>
+  </si>
+  <si>
+    <t>Se continua los pasos al ingresar una cuenta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +516,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -633,21 +666,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -664,6 +682,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -946,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,659 +992,695 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
     <col min="11" max="11" width="25.140625" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
     <col min="13" max="13" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="N8" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="9" t="s">
+      <c r="F11" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="9" t="s">
+      <c r="H13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="G23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="H23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="I23" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="J23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="K23" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1625,7 +1694,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1639,7 +1708,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1653,7 +1722,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1667,7 +1736,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1681,7 +1750,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1695,7 +1764,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1709,7 +1778,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1723,7 +1792,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1768,15 +1837,16 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ultimos cambios y nuevos archivos bugs e informe de bug
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoFinal-MariaCelesteParedes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFE7C96-7F85-45A2-A17F-7092D92DDFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B5734-AEF4-4475-A95E-EE82A975A96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="181">
   <si>
     <t>ID</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Usuario logueado, con una foto en la galería lista para publicar.</t>
   </si>
   <si>
-    <t>Foto: img_vacaciones.jpg, Descripción: "Gran día en la playa!"</t>
-  </si>
-  <si>
     <t>Publicación de foto simple con texto.</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>El video corto debe aparecer en el feed del usuario y reproducirse correctamente.</t>
   </si>
   <si>
-    <t>Intento de Selección Múltiple (Negativo)</t>
-  </si>
-  <si>
     <t>Verificar que el sistema NO permite la selección de más de un elemento (foto o video) para la publicación simultánea.</t>
   </si>
   <si>
@@ -270,21 +264,12 @@
     <t>Usuario logueado, publicación visible en el feed, la publicación NO debe tener un 'Me Gusta' previo del usuario.</t>
   </si>
   <si>
-    <t>Publicación ID: P-001</t>
-  </si>
-  <si>
     <t>Acción de "Me Gusta" inicial.</t>
   </si>
   <si>
-    <t>1. Localizar publicación P-001. 2. Tocar el icono de corazón (vacío).</t>
-  </si>
-  <si>
     <t>El contador de "Me Gusta" debe aumentar en una unidad, y el icono debe cambiar de vacío (blanco) a lleno (rojo).</t>
   </si>
   <si>
-    <t>Eliminar 'Me Gusta' (Dislike)</t>
-  </si>
-  <si>
     <t>Verificar que al volver a tocar el icono, se elimine el 'Me Gusta' y el contador disminuya.</t>
   </si>
   <si>
@@ -300,27 +285,18 @@
     <t>El contador de "Me Gusta" debe disminuir en una unidad, y el icono debe volver a su estado vacío (blanco).</t>
   </si>
   <si>
-    <t>Doble 'Me Gusta' (Validación de Estado)</t>
-  </si>
-  <si>
     <t>Verificar que el sistema mantenga un solo 'Me Gusta' aunque se toque el icono repetidamente.</t>
   </si>
   <si>
     <t>Usuario logueado, publicación sin 'Me Gusta' previo del usuario.</t>
   </si>
   <si>
-    <t>Publicación ID: P-002</t>
-  </si>
-  <si>
     <t>Estado estable del contador.</t>
   </si>
   <si>
     <t>1. Localizar publicación P-002. 2. Tocar el icono de corazón (vacío). 3. Tocar el icono de corazón (rojo/lleno) inmediatamente de nuevo.</t>
   </si>
   <si>
-    <t>El contador de "Me Gusta" debe aumentar en 1 en el primer toque y luego volver al conteo original en el segundo toque (neto: 0 cambios).</t>
-  </si>
-  <si>
     <t>Guardar Publicación por Primera Vez</t>
   </si>
   <si>
@@ -333,15 +309,9 @@
     <t>Usuario logueado, publicación visible en el feed, la publicación NO debe estar guardada previamente.</t>
   </si>
   <si>
-    <t>Publicación ID: P-003</t>
-  </si>
-  <si>
     <t>Acción de "Guardar" inicial.</t>
   </si>
   <si>
-    <t>1. Localizar publicación P-003. 2. Tocar el icono de 'Guardar' (vacío).</t>
-  </si>
-  <si>
     <t>El icono de 'Guardar' debe cambiar de vacío a lleno (rojo), indicando que la publicación ha sido guardada.</t>
   </si>
   <si>
@@ -351,63 +321,33 @@
     <t>Verificar que una publicación guardada sea accesible en la sección de Publicaciones Guardadas del perfil.</t>
   </si>
   <si>
-    <t>Usuario logueado, Publicación ID: P-003 previamente guardada (CP11).</t>
-  </si>
-  <si>
     <t>Verificación de acceso a lista.</t>
   </si>
   <si>
     <t>1. Ir al perfil del usuario. 2. Acceder a la sección de "Publicaciones Guardadas". 3. Buscar la publicación P-003.</t>
   </si>
   <si>
-    <t>La publicación P-003 debe aparecer y ser visible dentro de la sección de Publicaciones Guardadas.</t>
-  </si>
-  <si>
     <t>Eliminar Publicación Guardada</t>
   </si>
   <si>
     <t>Verificar que al volver a tocar el icono de 'Guardar' se elimine el guardado y el icono cambie de estado.</t>
   </si>
   <si>
-    <t>Usuario logueado, Publicación ID: P-003 previamente guardada (icono rojo/lleno).</t>
-  </si>
-  <si>
     <t>Eliminación de "Guardar".</t>
   </si>
   <si>
-    <t>1. Localizar publicación P-003 (guardada). 2. Tocar el icono de 'Guardar' (rojo/lleno) nuevamente. 3. (Opcional) Verificar la sección de Guardadas.</t>
-  </si>
-  <si>
-    <t>El icono de 'Guardar' debe volver a su estado vacío, y la publicación P-003 debe desaparecer de la sección de Publicaciones Guardadas.</t>
-  </si>
-  <si>
-    <t>Velocidad de Guardado de Publicación (Performance)</t>
-  </si>
-  <si>
     <t>Rendimiento (Guardar)</t>
   </si>
   <si>
     <t>Verificar que la acción de guardar una publicación se realice de forma ágil.</t>
   </si>
   <si>
-    <t>Usuario logueado, publicación visible.</t>
-  </si>
-  <si>
-    <t>Publicación ID: P-004</t>
-  </si>
-  <si>
     <t>Tiempo de respuesta de la acción.</t>
   </si>
   <si>
-    <t>1. Localizar publicación P-004. 2. Tocar el icono de 'Guardar'. 3. Medir el tiempo hasta el cambio de estado del icono.</t>
-  </si>
-  <si>
     <t>El cambio de estado del icono de 'Guardar' (vacío a lleno) debe ser inmediato (perceptualmente ágil, ej. menos de 1 segundo).</t>
   </si>
   <si>
-    <t>Velocidad de Recuperación de Lista Guardada (Performance)</t>
-  </si>
-  <si>
     <t>Verificar que la lista de publicaciones guardadas se recupere de forma ágil.</t>
   </si>
   <si>
@@ -444,9 +384,6 @@
     <t>1. No debe existir una cuenta previamente registrada con el numero de prueba.</t>
   </si>
   <si>
-    <t>Numero de celular: 51+921297961  Contraseña: 324667</t>
-  </si>
-  <si>
     <t>1. Abrir la app. 2. Seleccionar "Registrarse". 3. Ingresar numero y Contraseña débil. 4. Presionar "Iniciar sesión".</t>
   </si>
   <si>
@@ -481,13 +418,163 @@
   </si>
   <si>
     <t>Se continua los pasos al ingresar una cuenta</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-004</t>
+  </si>
+  <si>
+    <t>Permite despues del mensaje de permiso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Descripción: "Que rico!!"</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-005</t>
+  </si>
+  <si>
+    <t>Numero de celular: 51+921297961  Contraseña: 324667 , usuario: 9742.mp</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selección Múltiple </t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-007</t>
+  </si>
+  <si>
+    <t>Si permite selección multiple</t>
+  </si>
+  <si>
+    <t>1. Localizar la primera publicación. Tocar el icono de corazón (vacío).</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar 'Me Gusta' </t>
+  </si>
+  <si>
+    <t>Primera publicación</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doble 'Me Gusta' </t>
+  </si>
+  <si>
+    <t>El contador de "Me Gusta" debe aumentar en 1 en el primer toque y luego volver al conteo original en el segundo toque.</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-010</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación. 2. Tocar el icono de 'Guardar' (vacío).</t>
+  </si>
+  <si>
+    <t>Publicación : https://www.instagram.com/reel/DP4CnVfiK8d/?igsh=MXZlZWxqODU0aDBoYw==</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-011</t>
+  </si>
+  <si>
+    <t>Usuario logueado, Publicación :https://www.instagram.com/reel/DP4CnVfiK8d/?igsh=MXZlZWxqODU0aDBoYw==.</t>
+  </si>
+  <si>
+    <t>La publicación debe aparecer y ser visible dentro de la sección de Publicaciones Guardadas.</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-012</t>
+  </si>
+  <si>
+    <t>1. Localizar publicación  (guardada). 2. Tocar el icono de 'Guardar' (rojo/lleno) nuevamente. 3. (Opcional) Verificar la sección de Guardadas.</t>
+  </si>
+  <si>
+    <t>El icono de 'Guardar' debe volver a su estado vacío, y la publicación debe desaparecer de la sección de Publicaciones Guardadas.</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad de Guardado de Publicación </t>
+  </si>
+  <si>
+    <t>1. Localizar publicación. 2. Tocar el icono de 'Guardar'. 3. Medir el tiempo hasta el cambio de estado del icono.</t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-014</t>
+  </si>
+  <si>
+    <t>Usuario logueado, publicación visible: https://www.instagram.com/reel/DQRVOt7DrBA/?igsh=bG5uMWpzb2ZlYzh2</t>
+  </si>
+  <si>
+    <t>Publicación ID:https://www.instagram.com/reel/DQRVOt7DrBA/?igsh=bG5uMWpzb2ZlYzh2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad de Recuperación de Lista Guardada </t>
+  </si>
+  <si>
+    <t>EVIDENCIA TC-015</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Resumen de Resultados</t>
+  </si>
+  <si>
+    <t>Estado Requerido</t>
+  </si>
+  <si>
+    <t>Estado en la Fuente</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>OK / PASA</t>
+  </si>
+  <si>
+    <t>FAIL / NO PASA</t>
+  </si>
+  <si>
+    <t>BLOQUEADO</t>
+  </si>
+  <si>
+    <t>(No se registra)</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Porcentaje (%)</t>
+  </si>
+  <si>
+    <t>Bugs Críticos (Alta)</t>
+  </si>
+  <si>
+    <t>Bugs No Críticos</t>
+  </si>
+  <si>
+    <t>Bugs encontrados y severidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +610,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -538,7 +652,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -654,11 +768,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -699,11 +924,287 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -714,6 +1215,1248 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0"/>
+          <c:y val="0"/>
+          <c:w val="1"/>
+          <c:h val="1"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2BBE-40FC-AE9F-216FC69E2240}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-2BBE-40FC-AE9F-216FC69E2240}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-PE"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2BBE-40FC-AE9F-216FC69E2240}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-PE"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-2BBE-40FC-AE9F-216FC69E2240}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$38:$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Bugs Críticos (Alta)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bugs No Críticos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$38:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>33.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2BBE-40FC-AE9F-216FC69E2240}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredPieSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$C$37</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Cantidad</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:dPt>
+                  <c:idx val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                        <a:prstClr val="black">
+                          <a:alpha val="10000"/>
+                        </a:prstClr>
+                      </a:outerShdw>
+                    </a:effectLst>
+                    <a:scene3d>
+                      <a:camera prst="orthographicFront"/>
+                      <a:lightRig rig="threePt" dir="t"/>
+                    </a:scene3d>
+                    <a:sp3d>
+                      <a:bevelT w="127000" h="127000"/>
+                      <a:bevelB w="127000" h="127000"/>
+                    </a:sp3d>
+                  </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000005-2BBE-40FC-AE9F-216FC69E2240}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="1"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                        <a:prstClr val="black">
+                          <a:alpha val="10000"/>
+                        </a:prstClr>
+                      </a:outerShdw>
+                    </a:effectLst>
+                    <a:scene3d>
+                      <a:camera prst="orthographicFront"/>
+                      <a:lightRig rig="threePt" dir="t"/>
+                    </a:scene3d>
+                    <a:sp3d>
+                      <a:bevelT w="127000" h="127000"/>
+                      <a:bevelB w="127000" h="127000"/>
+                    </a:sp3d>
+                  </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000006-2BBE-40FC-AE9F-216FC69E2240}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dLbls>
+                  <c:dLbl>
+                    <c:idx val="0"/>
+                    <c:spPr>
+                      <a:noFill/>
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                    <c:txPr>
+                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                        <a:spAutoFit/>
+                      </a:bodyPr>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr>
+                          <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent1"/>
+                            </a:solidFill>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:defRPr>
+                        </a:pPr>
+                        <a:endParaRPr lang="es-PE"/>
+                      </a:p>
+                    </c:txPr>
+                    <c:dLblPos val="outEnd"/>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="0"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="1"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst>
+                      <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                        <c16:uniqueId val="{00000005-2BBE-40FC-AE9F-216FC69E2240}"/>
+                      </c:ext>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLbl>
+                    <c:idx val="1"/>
+                    <c:spPr>
+                      <a:noFill/>
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                    <c:txPr>
+                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                        <a:spAutoFit/>
+                      </a:bodyPr>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr>
+                          <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent2"/>
+                            </a:solidFill>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:defRPr>
+                        </a:pPr>
+                        <a:endParaRPr lang="es-PE"/>
+                      </a:p>
+                    </c:txPr>
+                    <c:dLblPos val="outEnd"/>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="0"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="1"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst>
+                      <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                        <c16:uniqueId val="{00000006-2BBE-40FC-AE9F-216FC69E2240}"/>
+                      </c:ext>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="1"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="1"/>
+                  <c:leaderLines>
+                    <c:spPr>
+                      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="35000"/>
+                            <a:lumOff val="65000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:round/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                  </c:leaderLines>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$B$38:$B$39</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Bugs Críticos (Alta)</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Bugs No Críticos</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$C$38:$C$39</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-2BBE-40FC-AE9F-216FC69E2240}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredPieSeries>
+          </c:ext>
+        </c:extLst>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1421946</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>16329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>81644</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E816D17-7B44-4CE7-86D4-F9A5FD5BBF6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F864A830-620C-4307-895E-C9BD2811083C}" name="Tabla1" displayName="Tabla1" ref="B37:D39" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="B37:D39" xr:uid="{F864A830-620C-4307-895E-C9BD2811083C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00142060-8FF0-473E-B003-2E6044DBAE50}" name="Categoría" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{ECF43B81-3906-4284-91F4-00A7CC3CE8CD}" name="Cantidad" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F9FC0C86-33E0-4A7B-BBA7-7479B1353B94}" name="Porcentaje (%)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,10 +2722,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N34"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,13 +2746,13 @@
     <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" customWidth="1"/>
     <col min="11" max="11" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="12" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:14" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
@@ -1015,7 +2763,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +2774,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
@@ -1037,7 +2785,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
@@ -1048,8 +2796,8 @@
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1086,19 +2834,22 @@
       <c r="L8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="O8" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>39</v>
@@ -1110,7 +2861,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>36</v>
@@ -1128,33 +2879,36 @@
         <v>44</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>134</v>
+        <v>113</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>165</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>36</v>
@@ -1166,27 +2920,30 @@
         <v>42</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>39</v>
@@ -1198,7 +2955,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>37</v>
@@ -1210,22 +2967,25 @@
         <v>47</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>48</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1259,11 +3019,20 @@
       <c r="K12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="L12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1280,7 +3049,7 @@
         <v>58</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>36</v>
@@ -1289,36 +3058,43 @@
         <v>37</v>
       </c>
       <c r="I13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="L13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>37</v>
@@ -1327,36 +3103,43 @@
         <v>37</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="L14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>37</v>
@@ -1365,35 +3148,45 @@
         <v>38</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="L15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>36</v>
@@ -1402,36 +3195,43 @@
         <v>37</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>36</v>
@@ -1440,36 +3240,43 @@
         <v>37</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>37</v>
@@ -1478,36 +3285,43 @@
         <v>38</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>36</v>
@@ -1516,36 +3330,43 @@
         <v>37</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>36</v>
@@ -1554,36 +3375,43 @@
         <v>37</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>37</v>
@@ -1592,36 +3420,43 @@
         <v>37</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>37</v>
@@ -1630,33 +3465,40 @@
         <v>38</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>46</v>
@@ -1668,19 +3510,26 @@
         <v>38</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1693,8 +3542,9 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1707,8 +3557,9 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1721,11 +3572,12 @@
       <c r="K26" s="2"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="16" t="s">
+        <v>167</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1735,11 +3587,9 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1749,11 +3599,18 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>170</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1763,11 +3620,18 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="18">
+        <v>12</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1777,11 +3641,18 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="18">
+        <v>3</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1791,11 +3662,18 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="18">
+        <v>0</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1805,8 +3683,9 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1819,8 +3698,9 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1834,9 +3714,71 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C35" s="23"/>
+    </row>
+    <row r="36" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="22"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="24">
+        <v>1</v>
+      </c>
+      <c r="D38" s="26">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="31">
+        <v>2</v>
+      </c>
+      <c r="D39" s="32">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+    </row>
+    <row r="41" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="21"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B42" s="20"/>
+    </row>
+    <row r="43" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="21"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="20"/>
+    </row>
+    <row r="45" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B45" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="A2:B2"/>
@@ -1847,7 +3789,34 @@
     <mergeCell ref="C4:E4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <conditionalFormatting sqref="M9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",M9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",M1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",M1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="27" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>